<commit_message>
Moved Video to useage bullets, as they were breaking in the screenshots section.
</commit_message>
<xml_diff>
--- a/Questionnair-Awnsers.xlsx
+++ b/Questionnair-Awnsers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\School\challengeAssignments\readme-generating-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB7D07A0-334D-4C10-B7DB-54518084AA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F8DDD3-F77E-4C09-BAF5-243A6EAF9036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{EDC773A3-FD11-4117-A105-4F5A4993C39B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>garrettWinter</t>
   </si>
@@ -158,13 +158,7 @@
     <t>No third parties followed but wanted to show functionality.</t>
   </si>
   <si>
-    <t>Video Demo of Application</t>
-  </si>
-  <si>
-    <t>https://garrettwinter.github.io/readme-generating-questionnaire/assets/media/README-Questionnair-Video.webm</t>
-  </si>
-  <si>
-    <t>VIDEO</t>
+    <t>Video Demo of Application - https://garrettwinter.github.io/readme-generating-questionnaire/assets/media/README-Questionnair-Video.webm</t>
   </si>
 </sst>
 </file>
@@ -529,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD1BC8F-F3DD-4B9B-8EDE-D32812007211}">
-  <dimension ref="A2:C41"/>
+  <dimension ref="A2:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,17 +631,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -655,7 +649,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
@@ -663,7 +657,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
@@ -671,24 +665,24 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
@@ -696,47 +690,47 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>13</v>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>14</v>
@@ -744,38 +738,30 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>